<commit_message>
fixup xlsx to json conversion for year
</commit_message>
<xml_diff>
--- a/scripts/files/updated_timeline.xlsx
+++ b/scripts/files/updated_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccahong/programming/soe-centennial-nextjs/scripts/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD32DF52-E76C-1345-A452-EEBC72B3DA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE80041-B5D2-C949-8E39-04CC5B013FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>year</t>
-  </si>
-  <si>
-    <t>headline</t>
   </si>
   <si>
     <t>alt</t>
@@ -1962,6 +1959,9 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/duv7bozlj/image/upload/v1741727933/harris_j_ryan_gw6by8.jpg</t>
+  </si>
+  <si>
+    <t>heading</t>
   </si>
 </sst>
 </file>
@@ -2352,7 +2352,7 @@
   <dimension ref="A1:E159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2365,2696 +2365,2696 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>632</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1925</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>1926</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>1926</v>
       </c>
       <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>1926</v>
       </c>
       <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>1926</v>
       </c>
       <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>1926</v>
       </c>
       <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>36</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>1926</v>
       </c>
       <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>40</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11">
         <v>1926</v>
       </c>
       <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12">
         <v>1927</v>
       </c>
       <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
         <v>47</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13">
         <v>1927</v>
       </c>
       <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>1972</v>
       </c>
       <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" t="s">
-        <v>56</v>
-      </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
         <v>57</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>59</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>60</v>
-      </c>
-      <c r="E15" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
         <v>62</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>63</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>64</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>65</v>
-      </c>
-      <c r="E16" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17">
         <v>1936</v>
       </c>
       <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
         <v>68</v>
       </c>
-      <c r="D17" t="s">
-        <v>69</v>
-      </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18">
         <v>1938</v>
       </c>
       <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
         <v>71</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>72</v>
-      </c>
-      <c r="E18" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19">
         <v>1937</v>
       </c>
       <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
         <v>75</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>76</v>
-      </c>
-      <c r="E19" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20">
         <v>1939</v>
       </c>
       <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
         <v>79</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>80</v>
-      </c>
-      <c r="E20" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21">
         <v>1939</v>
       </c>
       <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
         <v>83</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>84</v>
-      </c>
-      <c r="E21" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B22">
         <v>1939</v>
       </c>
       <c r="C22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" t="s">
         <v>87</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>88</v>
-      </c>
-      <c r="E22" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23">
         <v>1939</v>
       </c>
       <c r="C23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" t="s">
         <v>91</v>
       </c>
-      <c r="D23" t="s">
-        <v>92</v>
-      </c>
       <c r="E23" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24">
         <v>1942</v>
       </c>
       <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" t="s">
         <v>94</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>95</v>
-      </c>
-      <c r="E24" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
         <v>97</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>98</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>99</v>
-      </c>
-      <c r="E25" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26">
         <v>1939</v>
       </c>
       <c r="C26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" t="s">
         <v>102</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>103</v>
-      </c>
-      <c r="E26" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27">
         <v>1940</v>
       </c>
       <c r="C27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" t="s">
         <v>106</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>107</v>
-      </c>
-      <c r="E27" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28">
         <v>1943</v>
       </c>
       <c r="C28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" t="s">
         <v>110</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>111</v>
-      </c>
-      <c r="E28" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29">
         <v>1943</v>
       </c>
       <c r="C29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" t="s">
         <v>114</v>
       </c>
-      <c r="D29" t="s">
-        <v>115</v>
-      </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B30">
         <v>1944</v>
       </c>
       <c r="C30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" t="s">
         <v>117</v>
       </c>
-      <c r="D30" t="s">
-        <v>118</v>
-      </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B31">
         <v>1944</v>
       </c>
       <c r="C31" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" t="s">
         <v>120</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>121</v>
-      </c>
-      <c r="E31" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32">
         <v>1944</v>
       </c>
       <c r="C32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" t="s">
         <v>124</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>125</v>
-      </c>
-      <c r="E32" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" t="s">
         <v>127</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>128</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>129</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>130</v>
-      </c>
-      <c r="E33" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" t="s">
         <v>132</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>133</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>134</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>135</v>
-      </c>
-      <c r="E34" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B35">
         <v>1947</v>
       </c>
       <c r="C35" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" t="s">
         <v>138</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>139</v>
-      </c>
-      <c r="E35" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B36">
         <v>1949</v>
       </c>
       <c r="C36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" t="s">
         <v>142</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>143</v>
-      </c>
-      <c r="E36" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B37">
         <v>1952</v>
       </c>
       <c r="C37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" t="s">
         <v>146</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>147</v>
-      </c>
-      <c r="E37" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B38">
         <v>1950</v>
       </c>
       <c r="C38" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" t="s">
         <v>150</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>151</v>
-      </c>
-      <c r="E38" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B39">
         <v>1948</v>
       </c>
       <c r="C39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" t="s">
         <v>154</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>155</v>
-      </c>
-      <c r="E39" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B40">
         <v>1951</v>
       </c>
       <c r="C40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" t="s">
         <v>158</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>159</v>
-      </c>
-      <c r="E40" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B41">
         <v>1953</v>
       </c>
       <c r="C41" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" t="s">
         <v>162</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>163</v>
-      </c>
-      <c r="E41" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B42">
         <v>1952</v>
       </c>
       <c r="C42" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" t="s">
         <v>166</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>167</v>
-      </c>
-      <c r="E42" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B43">
         <v>1951</v>
       </c>
       <c r="C43" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" t="s">
         <v>170</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>171</v>
-      </c>
-      <c r="E43" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>172</v>
+      </c>
+      <c r="B44" t="s">
         <v>173</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>174</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>175</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>176</v>
-      </c>
-      <c r="E44" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B45">
         <v>1955</v>
       </c>
       <c r="C45" t="s">
+        <v>178</v>
+      </c>
+      <c r="D45" t="s">
         <v>179</v>
       </c>
-      <c r="D45" t="s">
-        <v>180</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>180</v>
+      </c>
+      <c r="B46" t="s">
         <v>181</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>182</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" t="s">
         <v>183</v>
-      </c>
-      <c r="D46" t="s">
-        <v>65</v>
-      </c>
-      <c r="E46" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B47">
         <v>1963</v>
       </c>
       <c r="C47" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" t="s">
         <v>186</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>187</v>
-      </c>
-      <c r="E47" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B48">
         <v>1958</v>
       </c>
       <c r="C48" t="s">
+        <v>189</v>
+      </c>
+      <c r="D48" t="s">
         <v>190</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>191</v>
-      </c>
-      <c r="E48" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B49">
         <v>1959</v>
       </c>
       <c r="C49" t="s">
+        <v>193</v>
+      </c>
+      <c r="D49" t="s">
         <v>194</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>195</v>
-      </c>
-      <c r="E49" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B50">
         <v>1961</v>
       </c>
       <c r="C50" t="s">
+        <v>197</v>
+      </c>
+      <c r="D50" t="s">
         <v>198</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>199</v>
-      </c>
-      <c r="E50" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B51">
         <v>1963</v>
       </c>
       <c r="C51" t="s">
+        <v>201</v>
+      </c>
+      <c r="D51" t="s">
         <v>202</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>203</v>
-      </c>
-      <c r="E51" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B52">
         <v>1964</v>
       </c>
       <c r="C52" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" t="s">
         <v>206</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>207</v>
-      </c>
-      <c r="E52" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B53">
         <v>1954</v>
       </c>
       <c r="C53" t="s">
+        <v>209</v>
+      </c>
+      <c r="D53" t="s">
         <v>210</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>211</v>
-      </c>
-      <c r="E53" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B54">
         <v>1962</v>
       </c>
       <c r="C54" t="s">
+        <v>213</v>
+      </c>
+      <c r="D54" t="s">
         <v>214</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>215</v>
-      </c>
-      <c r="E54" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B55">
         <v>1955</v>
       </c>
       <c r="C55" t="s">
+        <v>217</v>
+      </c>
+      <c r="D55" t="s">
         <v>218</v>
       </c>
-      <c r="D55" t="s">
-        <v>219</v>
-      </c>
       <c r="E55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B56">
         <v>1966</v>
       </c>
       <c r="C56" t="s">
+        <v>220</v>
+      </c>
+      <c r="D56" t="s">
         <v>221</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>222</v>
-      </c>
-      <c r="E56" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B57">
         <v>1961</v>
       </c>
       <c r="C57" t="s">
+        <v>224</v>
+      </c>
+      <c r="D57" t="s">
         <v>225</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>226</v>
-      </c>
-      <c r="E57" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B58">
         <v>1958</v>
       </c>
       <c r="C58" t="s">
+        <v>228</v>
+      </c>
+      <c r="D58" t="s">
         <v>229</v>
       </c>
-      <c r="D58" t="s">
-        <v>230</v>
-      </c>
       <c r="E58" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B59">
         <v>1963</v>
       </c>
       <c r="C59" t="s">
+        <v>231</v>
+      </c>
+      <c r="D59" t="s">
         <v>232</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>233</v>
-      </c>
-      <c r="E59" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B60">
         <v>1965</v>
       </c>
       <c r="C60" t="s">
+        <v>235</v>
+      </c>
+      <c r="D60" t="s">
         <v>236</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>237</v>
-      </c>
-      <c r="E60" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B61">
         <v>1965</v>
       </c>
       <c r="C61" t="s">
+        <v>239</v>
+      </c>
+      <c r="D61" t="s">
         <v>240</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>241</v>
-      </c>
-      <c r="E61" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B62">
         <v>1972</v>
       </c>
       <c r="C62" t="s">
+        <v>243</v>
+      </c>
+      <c r="D62" t="s">
         <v>244</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>245</v>
-      </c>
-      <c r="E62" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B63">
         <v>1969</v>
       </c>
       <c r="C63" t="s">
+        <v>247</v>
+      </c>
+      <c r="D63" t="s">
         <v>248</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>249</v>
-      </c>
-      <c r="E63" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B64">
         <v>1966</v>
       </c>
       <c r="C64" t="s">
+        <v>251</v>
+      </c>
+      <c r="D64" t="s">
         <v>252</v>
       </c>
-      <c r="D64" t="s">
-        <v>253</v>
-      </c>
       <c r="E64" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B65">
         <v>1973</v>
       </c>
       <c r="C65" t="s">
+        <v>254</v>
+      </c>
+      <c r="D65" t="s">
         <v>255</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>256</v>
-      </c>
-      <c r="E65" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B66">
         <v>1975</v>
       </c>
       <c r="C66" t="s">
+        <v>258</v>
+      </c>
+      <c r="D66" t="s">
         <v>259</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>260</v>
-      </c>
-      <c r="E66" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B67">
         <v>1974</v>
       </c>
       <c r="C67" t="s">
+        <v>262</v>
+      </c>
+      <c r="D67" t="s">
         <v>263</v>
       </c>
-      <c r="D67" t="s">
-        <v>264</v>
-      </c>
       <c r="E67" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B68">
         <v>1969</v>
       </c>
       <c r="C68" t="s">
+        <v>265</v>
+      </c>
+      <c r="D68" t="s">
         <v>266</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>267</v>
-      </c>
-      <c r="E68" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B69">
         <v>1971</v>
       </c>
       <c r="C69" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D69" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E69" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>270</v>
+      </c>
+      <c r="B70" t="s">
         <v>271</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>272</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>273</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>274</v>
-      </c>
-      <c r="E70" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B71">
         <v>1969</v>
       </c>
       <c r="C71" t="s">
+        <v>276</v>
+      </c>
+      <c r="D71" t="s">
         <v>277</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>278</v>
-      </c>
-      <c r="E71" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B72">
         <v>1968</v>
       </c>
       <c r="C72" t="s">
+        <v>280</v>
+      </c>
+      <c r="D72" t="s">
         <v>281</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>282</v>
-      </c>
-      <c r="E72" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B73">
         <v>1972</v>
       </c>
       <c r="C73" t="s">
+        <v>284</v>
+      </c>
+      <c r="D73" t="s">
         <v>285</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>286</v>
-      </c>
-      <c r="E73" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B74">
         <v>1972</v>
       </c>
       <c r="C74" t="s">
+        <v>288</v>
+      </c>
+      <c r="D74" t="s">
+        <v>285</v>
+      </c>
+      <c r="E74" t="s">
         <v>289</v>
-      </c>
-      <c r="D74" t="s">
-        <v>286</v>
-      </c>
-      <c r="E74" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B75">
         <v>1972</v>
       </c>
       <c r="C75" t="s">
+        <v>291</v>
+      </c>
+      <c r="D75" t="s">
         <v>292</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>293</v>
-      </c>
-      <c r="E75" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B76">
         <v>1974</v>
       </c>
       <c r="C76" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D76" t="s">
+        <v>248</v>
+      </c>
+      <c r="E76" t="s">
         <v>249</v>
-      </c>
-      <c r="E76" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B77">
         <v>1975</v>
       </c>
       <c r="C77" t="s">
+        <v>297</v>
+      </c>
+      <c r="D77" t="s">
         <v>298</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>299</v>
-      </c>
-      <c r="E77" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B78">
         <v>1974</v>
       </c>
       <c r="C78" t="s">
+        <v>301</v>
+      </c>
+      <c r="D78" t="s">
         <v>302</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>303</v>
-      </c>
-      <c r="E78" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B79">
         <v>1972</v>
       </c>
       <c r="C79" t="s">
+        <v>305</v>
+      </c>
+      <c r="D79" t="s">
         <v>306</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>307</v>
-      </c>
-      <c r="E79" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B80">
         <v>1978</v>
       </c>
       <c r="C80" t="s">
+        <v>309</v>
+      </c>
+      <c r="D80" t="s">
         <v>310</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>311</v>
-      </c>
-      <c r="E80" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B81">
         <v>1983</v>
       </c>
       <c r="C81" t="s">
+        <v>313</v>
+      </c>
+      <c r="D81" t="s">
         <v>314</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>315</v>
-      </c>
-      <c r="E81" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B82">
         <v>1977</v>
       </c>
       <c r="C82" t="s">
+        <v>317</v>
+      </c>
+      <c r="D82" t="s">
         <v>318</v>
       </c>
-      <c r="D82" t="s">
-        <v>319</v>
-      </c>
       <c r="E82" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B83">
         <v>1977</v>
       </c>
       <c r="C83" t="s">
+        <v>320</v>
+      </c>
+      <c r="D83" t="s">
         <v>321</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>322</v>
-      </c>
-      <c r="E83" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B84">
         <v>1977</v>
       </c>
       <c r="C84" t="s">
+        <v>324</v>
+      </c>
+      <c r="D84" t="s">
         <v>325</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>326</v>
-      </c>
-      <c r="E84" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B85">
         <v>1981</v>
       </c>
       <c r="C85" t="s">
+        <v>328</v>
+      </c>
+      <c r="D85" t="s">
         <v>329</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>330</v>
-      </c>
-      <c r="E85" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B86">
         <v>1984</v>
       </c>
       <c r="C86" t="s">
+        <v>332</v>
+      </c>
+      <c r="D86" t="s">
         <v>333</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>334</v>
-      </c>
-      <c r="E86" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B87">
         <v>1984</v>
       </c>
       <c r="C87" t="s">
+        <v>336</v>
+      </c>
+      <c r="D87" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" t="s">
         <v>337</v>
-      </c>
-      <c r="D87" t="s">
-        <v>17</v>
-      </c>
-      <c r="E87" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B88">
         <v>1989</v>
       </c>
       <c r="C88" t="s">
+        <v>339</v>
+      </c>
+      <c r="D88" t="s">
         <v>340</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>341</v>
-      </c>
-      <c r="E88" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B89">
         <v>1985</v>
       </c>
       <c r="C89" t="s">
+        <v>343</v>
+      </c>
+      <c r="D89" t="s">
         <v>344</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>345</v>
-      </c>
-      <c r="E89" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>346</v>
+      </c>
+      <c r="B90" t="s">
         <v>347</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>348</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>349</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>350</v>
-      </c>
-      <c r="E90" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B91">
         <v>1994</v>
       </c>
       <c r="C91" t="s">
+        <v>352</v>
+      </c>
+      <c r="D91" t="s">
         <v>353</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>354</v>
-      </c>
-      <c r="E91" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B92">
         <v>1994</v>
       </c>
       <c r="C92" t="s">
+        <v>356</v>
+      </c>
+      <c r="D92" t="s">
         <v>357</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>358</v>
-      </c>
-      <c r="E92" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B93">
         <v>1996</v>
       </c>
       <c r="C93" t="s">
+        <v>360</v>
+      </c>
+      <c r="D93" t="s">
         <v>361</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>362</v>
-      </c>
-      <c r="E93" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B94">
         <v>1992</v>
       </c>
       <c r="C94" t="s">
+        <v>364</v>
+      </c>
+      <c r="D94" t="s">
         <v>365</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>366</v>
-      </c>
-      <c r="E94" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B95">
         <v>1993</v>
       </c>
       <c r="C95" t="s">
+        <v>368</v>
+      </c>
+      <c r="D95" t="s">
         <v>369</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>370</v>
-      </c>
-      <c r="E95" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B96">
         <v>1993</v>
       </c>
       <c r="C96" t="s">
+        <v>372</v>
+      </c>
+      <c r="D96" t="s">
         <v>373</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>374</v>
-      </c>
-      <c r="E96" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B97">
         <v>1989</v>
       </c>
       <c r="C97" t="s">
+        <v>376</v>
+      </c>
+      <c r="D97" t="s">
         <v>377</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>378</v>
-      </c>
-      <c r="E97" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B98">
         <v>1989</v>
       </c>
       <c r="C98" t="s">
+        <v>380</v>
+      </c>
+      <c r="D98" t="s">
         <v>381</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>382</v>
-      </c>
-      <c r="E98" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B99">
         <v>1994</v>
       </c>
       <c r="C99" t="s">
+        <v>384</v>
+      </c>
+      <c r="D99" t="s">
         <v>385</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>386</v>
-      </c>
-      <c r="E99" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B100">
         <v>1994</v>
       </c>
       <c r="C100" t="s">
+        <v>388</v>
+      </c>
+      <c r="D100" t="s">
         <v>389</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>390</v>
-      </c>
-      <c r="E100" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B101">
         <v>2000</v>
       </c>
       <c r="C101" t="s">
+        <v>392</v>
+      </c>
+      <c r="D101" t="s">
         <v>393</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>394</v>
-      </c>
-      <c r="E101" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B102">
         <v>1996</v>
       </c>
       <c r="C102" t="s">
+        <v>396</v>
+      </c>
+      <c r="D102" t="s">
         <v>397</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
         <v>398</v>
-      </c>
-      <c r="E102" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B103">
         <v>2005</v>
       </c>
       <c r="C103" t="s">
+        <v>400</v>
+      </c>
+      <c r="D103" t="s">
         <v>401</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>402</v>
-      </c>
-      <c r="E103" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B104">
         <v>1996</v>
       </c>
       <c r="C104" t="s">
+        <v>404</v>
+      </c>
+      <c r="D104" t="s">
         <v>405</v>
       </c>
-      <c r="D104" t="s">
+      <c r="E104" t="s">
         <v>406</v>
-      </c>
-      <c r="E104" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B105">
         <v>2022</v>
       </c>
       <c r="C105" t="s">
+        <v>408</v>
+      </c>
+      <c r="D105" t="s">
         <v>409</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>410</v>
-      </c>
-      <c r="E105" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B106">
         <v>1996</v>
       </c>
       <c r="C106" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D106" t="s">
+        <v>412</v>
+      </c>
+      <c r="E106" t="s">
         <v>413</v>
-      </c>
-      <c r="E106" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>414</v>
+      </c>
+      <c r="B107" t="s">
         <v>415</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>416</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
         <v>417</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E107" t="s">
         <v>418</v>
-      </c>
-      <c r="E107" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B108">
         <v>2005</v>
       </c>
       <c r="C108" t="s">
+        <v>420</v>
+      </c>
+      <c r="D108" t="s">
         <v>421</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E108" t="s">
         <v>422</v>
-      </c>
-      <c r="E108" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B109">
         <v>1992</v>
       </c>
       <c r="C109" t="s">
+        <v>424</v>
+      </c>
+      <c r="D109" t="s">
         <v>425</v>
       </c>
-      <c r="D109" t="s">
+      <c r="E109" t="s">
         <v>426</v>
-      </c>
-      <c r="E109" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B110">
         <v>2022</v>
       </c>
       <c r="C110" t="s">
+        <v>428</v>
+      </c>
+      <c r="D110" t="s">
         <v>429</v>
       </c>
-      <c r="D110" t="s">
+      <c r="E110" t="s">
         <v>430</v>
-      </c>
-      <c r="E110" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B111">
         <v>2005</v>
       </c>
       <c r="C111" t="s">
+        <v>432</v>
+      </c>
+      <c r="D111" t="s">
         <v>433</v>
       </c>
-      <c r="D111" t="s">
+      <c r="E111" t="s">
         <v>434</v>
-      </c>
-      <c r="E111" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B112">
         <v>1996</v>
       </c>
       <c r="C112" t="s">
+        <v>436</v>
+      </c>
+      <c r="D112" t="s">
         <v>437</v>
       </c>
-      <c r="D112" t="s">
+      <c r="E112" t="s">
         <v>438</v>
-      </c>
-      <c r="E112" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B113">
         <v>1996</v>
       </c>
       <c r="C113" t="s">
+        <v>440</v>
+      </c>
+      <c r="D113" t="s">
         <v>441</v>
       </c>
-      <c r="D113" t="s">
+      <c r="E113" t="s">
         <v>442</v>
-      </c>
-      <c r="E113" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B114">
         <v>2003</v>
       </c>
       <c r="C114" t="s">
+        <v>444</v>
+      </c>
+      <c r="D114" t="s">
         <v>445</v>
       </c>
-      <c r="D114" t="s">
+      <c r="E114" t="s">
         <v>446</v>
-      </c>
-      <c r="E114" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B115">
         <v>2004</v>
       </c>
       <c r="C115" t="s">
+        <v>448</v>
+      </c>
+      <c r="D115" t="s">
         <v>449</v>
       </c>
-      <c r="D115" t="s">
+      <c r="E115" t="s">
         <v>450</v>
-      </c>
-      <c r="E115" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B116">
         <v>2010</v>
       </c>
       <c r="C116" t="s">
+        <v>452</v>
+      </c>
+      <c r="D116" t="s">
         <v>453</v>
       </c>
-      <c r="D116" t="s">
+      <c r="E116" t="s">
         <v>454</v>
-      </c>
-      <c r="E116" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B117">
         <v>2006</v>
       </c>
       <c r="C117" t="s">
+        <v>456</v>
+      </c>
+      <c r="D117" t="s">
         <v>457</v>
       </c>
-      <c r="D117" t="s">
+      <c r="E117" t="s">
         <v>458</v>
-      </c>
-      <c r="E117" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B118">
         <v>2008</v>
       </c>
       <c r="C118" t="s">
+        <v>460</v>
+      </c>
+      <c r="D118" t="s">
         <v>461</v>
       </c>
-      <c r="D118" t="s">
+      <c r="E118" t="s">
         <v>462</v>
-      </c>
-      <c r="E118" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B119">
         <v>2010</v>
       </c>
       <c r="C119" t="s">
+        <v>464</v>
+      </c>
+      <c r="D119" t="s">
         <v>465</v>
       </c>
-      <c r="D119" t="s">
-        <v>466</v>
-      </c>
       <c r="E119" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B120">
         <v>2011</v>
       </c>
       <c r="C120" t="s">
+        <v>467</v>
+      </c>
+      <c r="D120" t="s">
         <v>468</v>
       </c>
-      <c r="D120" t="s">
+      <c r="E120" t="s">
         <v>469</v>
-      </c>
-      <c r="E120" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B121">
         <v>2014</v>
       </c>
       <c r="C121" t="s">
+        <v>471</v>
+      </c>
+      <c r="D121" t="s">
         <v>472</v>
       </c>
-      <c r="D121" t="s">
-        <v>473</v>
-      </c>
       <c r="E121" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B122">
         <v>2010</v>
       </c>
       <c r="C122" t="s">
+        <v>474</v>
+      </c>
+      <c r="D122" t="s">
         <v>475</v>
       </c>
-      <c r="D122" t="s">
+      <c r="E122" t="s">
         <v>476</v>
-      </c>
-      <c r="E122" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B123">
         <v>2014</v>
       </c>
       <c r="C123" t="s">
+        <v>478</v>
+      </c>
+      <c r="D123" t="s">
         <v>479</v>
       </c>
-      <c r="D123" t="s">
+      <c r="E123" t="s">
         <v>480</v>
-      </c>
-      <c r="E123" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B124">
         <v>2014</v>
       </c>
       <c r="C124" t="s">
+        <v>482</v>
+      </c>
+      <c r="D124" t="s">
         <v>483</v>
       </c>
-      <c r="D124" t="s">
+      <c r="E124" t="s">
         <v>484</v>
-      </c>
-      <c r="E124" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B125">
         <v>2011</v>
       </c>
       <c r="C125" t="s">
+        <v>486</v>
+      </c>
+      <c r="D125" t="s">
         <v>487</v>
       </c>
-      <c r="D125" t="s">
+      <c r="E125" t="s">
         <v>488</v>
-      </c>
-      <c r="E125" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>489</v>
+      </c>
+      <c r="B126" t="s">
         <v>490</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>491</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>492</v>
       </c>
-      <c r="D126" t="s">
+      <c r="E126" t="s">
         <v>493</v>
-      </c>
-      <c r="E126" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B127">
         <v>2014</v>
       </c>
       <c r="C127" t="s">
+        <v>495</v>
+      </c>
+      <c r="D127" t="s">
         <v>496</v>
       </c>
-      <c r="D127" t="s">
-        <v>497</v>
-      </c>
       <c r="E127" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B128">
         <v>2005</v>
       </c>
       <c r="C128" t="s">
+        <v>498</v>
+      </c>
+      <c r="D128" t="s">
         <v>499</v>
       </c>
-      <c r="D128" t="s">
+      <c r="E128" t="s">
         <v>500</v>
-      </c>
-      <c r="E128" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B129">
         <v>2005</v>
       </c>
       <c r="C129" t="s">
+        <v>502</v>
+      </c>
+      <c r="D129" t="s">
         <v>503</v>
       </c>
-      <c r="D129" t="s">
+      <c r="E129" t="s">
         <v>504</v>
-      </c>
-      <c r="E129" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B130">
         <v>2017</v>
       </c>
       <c r="C130" t="s">
+        <v>506</v>
+      </c>
+      <c r="D130" t="s">
         <v>507</v>
       </c>
-      <c r="D130" t="s">
+      <c r="E130" t="s">
         <v>508</v>
-      </c>
-      <c r="E130" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B131">
         <v>2012</v>
       </c>
       <c r="C131" t="s">
+        <v>510</v>
+      </c>
+      <c r="D131" t="s">
         <v>511</v>
       </c>
-      <c r="D131" t="s">
+      <c r="E131" t="s">
         <v>512</v>
-      </c>
-      <c r="E131" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B132">
         <v>2023</v>
       </c>
       <c r="C132" t="s">
+        <v>514</v>
+      </c>
+      <c r="D132" t="s">
         <v>515</v>
       </c>
-      <c r="D132" t="s">
+      <c r="E132" t="s">
         <v>516</v>
-      </c>
-      <c r="E132" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B133">
         <v>2014</v>
       </c>
       <c r="C133" t="s">
+        <v>518</v>
+      </c>
+      <c r="D133" t="s">
         <v>519</v>
       </c>
-      <c r="D133" t="s">
+      <c r="E133" t="s">
         <v>520</v>
-      </c>
-      <c r="E133" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B134">
         <v>2014</v>
       </c>
       <c r="C134" t="s">
+        <v>522</v>
+      </c>
+      <c r="D134" t="s">
         <v>523</v>
       </c>
-      <c r="D134" t="s">
+      <c r="E134" t="s">
         <v>524</v>
-      </c>
-      <c r="E134" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B135">
         <v>2022</v>
       </c>
       <c r="C135" t="s">
+        <v>526</v>
+      </c>
+      <c r="D135" t="s">
         <v>527</v>
       </c>
-      <c r="D135" t="s">
+      <c r="E135" t="s">
         <v>528</v>
-      </c>
-      <c r="E135" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B136">
         <v>2015</v>
       </c>
       <c r="C136" t="s">
+        <v>530</v>
+      </c>
+      <c r="D136" t="s">
         <v>531</v>
       </c>
-      <c r="D136" t="s">
+      <c r="E136" t="s">
         <v>532</v>
-      </c>
-      <c r="E136" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B137">
         <v>2017</v>
       </c>
       <c r="C137" t="s">
+        <v>534</v>
+      </c>
+      <c r="D137" t="s">
         <v>535</v>
       </c>
-      <c r="D137" t="s">
+      <c r="E137" t="s">
         <v>536</v>
-      </c>
-      <c r="E137" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B138">
         <v>2009</v>
       </c>
       <c r="C138" t="s">
+        <v>538</v>
+      </c>
+      <c r="D138" t="s">
         <v>539</v>
       </c>
-      <c r="D138" t="s">
+      <c r="E138" t="s">
         <v>540</v>
-      </c>
-      <c r="E138" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B139">
         <v>2023</v>
       </c>
       <c r="C139" t="s">
+        <v>542</v>
+      </c>
+      <c r="D139" t="s">
         <v>543</v>
       </c>
-      <c r="D139" t="s">
+      <c r="E139" t="s">
         <v>544</v>
-      </c>
-      <c r="E139" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B140">
         <v>2016</v>
       </c>
       <c r="C140" t="s">
+        <v>546</v>
+      </c>
+      <c r="D140" t="s">
         <v>547</v>
       </c>
-      <c r="D140" t="s">
+      <c r="E140" t="s">
         <v>548</v>
-      </c>
-      <c r="E140" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B141">
         <v>2018</v>
       </c>
       <c r="C141" t="s">
+        <v>550</v>
+      </c>
+      <c r="D141" t="s">
         <v>551</v>
       </c>
-      <c r="D141" t="s">
+      <c r="E141" t="s">
         <v>552</v>
-      </c>
-      <c r="E141" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B142">
         <v>2019</v>
       </c>
       <c r="C142" t="s">
+        <v>554</v>
+      </c>
+      <c r="D142" t="s">
         <v>555</v>
       </c>
-      <c r="D142" t="s">
+      <c r="E142" t="s">
         <v>556</v>
-      </c>
-      <c r="E142" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B143">
         <v>2024</v>
       </c>
       <c r="C143" t="s">
+        <v>558</v>
+      </c>
+      <c r="D143" t="s">
         <v>559</v>
       </c>
-      <c r="D143" t="s">
+      <c r="E143" t="s">
         <v>560</v>
-      </c>
-      <c r="E143" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B144">
         <v>2021</v>
       </c>
       <c r="C144" t="s">
+        <v>562</v>
+      </c>
+      <c r="D144" t="s">
         <v>563</v>
       </c>
-      <c r="D144" t="s">
+      <c r="E144" t="s">
         <v>564</v>
-      </c>
-      <c r="E144" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B145">
         <v>2020</v>
       </c>
       <c r="C145" t="s">
+        <v>566</v>
+      </c>
+      <c r="D145" t="s">
         <v>567</v>
       </c>
-      <c r="D145" t="s">
+      <c r="E145" t="s">
         <v>568</v>
-      </c>
-      <c r="E145" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B146">
         <v>1987</v>
       </c>
       <c r="C146" t="s">
+        <v>570</v>
+      </c>
+      <c r="D146" t="s">
         <v>571</v>
       </c>
-      <c r="D146" t="s">
+      <c r="E146" t="s">
         <v>572</v>
-      </c>
-      <c r="E146" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B147">
         <v>2021</v>
       </c>
       <c r="C147" t="s">
+        <v>574</v>
+      </c>
+      <c r="D147" t="s">
         <v>575</v>
       </c>
-      <c r="D147" t="s">
-        <v>576</v>
-      </c>
       <c r="E147" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>576</v>
+      </c>
+      <c r="B148" t="s">
         <v>577</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C148" t="s">
         <v>578</v>
       </c>
-      <c r="C148" t="s">
+      <c r="D148" t="s">
         <v>579</v>
       </c>
-      <c r="D148" t="s">
-        <v>580</v>
-      </c>
       <c r="E148" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B149">
         <v>2023</v>
       </c>
       <c r="C149" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D149" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E149" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B150">
         <v>2022</v>
       </c>
       <c r="C150" t="s">
+        <v>583</v>
+      </c>
+      <c r="D150" t="s">
         <v>584</v>
       </c>
-      <c r="D150" t="s">
+      <c r="E150" t="s">
         <v>585</v>
-      </c>
-      <c r="E150" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B151">
         <v>2022</v>
       </c>
       <c r="C151" t="s">
+        <v>587</v>
+      </c>
+      <c r="D151" t="s">
         <v>588</v>
       </c>
-      <c r="D151" t="s">
-        <v>589</v>
-      </c>
       <c r="E151" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B152">
         <v>2024</v>
       </c>
       <c r="C152" t="s">
+        <v>590</v>
+      </c>
+      <c r="D152" t="s">
         <v>591</v>
       </c>
-      <c r="D152" t="s">
-        <v>592</v>
-      </c>
       <c r="E152" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B153">
         <v>2016</v>
       </c>
       <c r="C153" t="s">
+        <v>593</v>
+      </c>
+      <c r="D153" t="s">
         <v>594</v>
       </c>
-      <c r="D153" t="s">
-        <v>595</v>
-      </c>
       <c r="E153" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B154">
         <v>2023</v>
       </c>
       <c r="C154" t="s">
+        <v>596</v>
+      </c>
+      <c r="D154" t="s">
         <v>597</v>
       </c>
-      <c r="D154" t="s">
+      <c r="E154" t="s">
         <v>598</v>
-      </c>
-      <c r="E154" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B155">
         <v>2023</v>
       </c>
       <c r="C155" t="s">
+        <v>600</v>
+      </c>
+      <c r="D155" t="s">
         <v>601</v>
       </c>
-      <c r="D155" t="s">
+      <c r="E155" t="s">
         <v>602</v>
-      </c>
-      <c r="E155" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B156">
         <v>2021</v>
       </c>
       <c r="C156" t="s">
+        <v>604</v>
+      </c>
+      <c r="D156" t="s">
         <v>605</v>
       </c>
-      <c r="D156" t="s">
+      <c r="E156" t="s">
         <v>606</v>
-      </c>
-      <c r="E156" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B157">
         <v>2025</v>
       </c>
       <c r="C157" t="s">
+        <v>608</v>
+      </c>
+      <c r="D157" t="s">
         <v>609</v>
       </c>
-      <c r="D157" t="s">
+      <c r="E157" t="s">
         <v>610</v>
-      </c>
-      <c r="E157" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B158">
         <v>2024</v>
       </c>
       <c r="C158" t="s">
+        <v>612</v>
+      </c>
+      <c r="D158" t="s">
         <v>613</v>
       </c>
-      <c r="D158" t="s">
+      <c r="E158" t="s">
         <v>614</v>
-      </c>
-      <c r="E158" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B159">
         <v>1970</v>
       </c>
       <c r="C159" t="s">
+        <v>616</v>
+      </c>
+      <c r="D159" t="s">
         <v>617</v>
       </c>
-      <c r="D159" t="s">
+      <c r="E159" t="s">
         <v>618</v>
-      </c>
-      <c r="E159" t="s">
-        <v>619</v>
       </c>
     </row>
   </sheetData>
@@ -5076,7 +5076,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D1 A2:D5 A16:D22 A32:D44 A46:D57 A60:D63 A77:D81 A88:D100 A101:D115 A116:D118 A135:D146 A148:D150 A147:D147 A154:D159 A151:D151 A152:D152 A153:D153 A128:D134 A127:D127 A122:D126 A121:D121 A120:D120 A119:D119 A83:D87 A82:D82 A68:D76 A67:D67 A65:D66 A64:D64 A59:D59 A58:D58 A45:D45 A24:D31 A23:D23 A7:D15 A6:D6 E1 E2:E5 E16:E22 E32:E44 E46:E57 E60:E63 E77:E81 E88:E100 E101:E115 E116:E118 E135:E146 E148:E150 E154:E159 E128:E134 E122:E126 E120 E83:E87 E68:E76 E65:E66 E59 E24:E31 E7:E15" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B1 A2:D5 A16:D22 A32:D44 A46:D57 A60:D63 A77:D81 A88:D100 A101:D115 A116:D118 A135:D146 A148:D150 A147:D147 A154:D159 A151:D151 A152:D152 A153:D153 A128:D134 A127:D127 A122:D126 A121:D121 A120:D120 A119:D119 A83:D87 A82:D82 A68:D76 A67:D67 A65:D66 A64:D64 A59:D59 A58:D58 A45:D45 A24:D31 A23:D23 A7:D15 A6:D6 E1 E2:E5 E16:E22 E32:E44 E46:E57 E60:E63 E77:E81 E88:E100 E101:E115 E116:E118 E135:E146 E148:E150 E154:E159 E128:E134 E122:E126 E120 E83:E87 E68:E76 E65:E66 E59 E24:E31 E7:E15 D1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>